<commit_message>
Update Croatia configuration and add new transformation strategies
</commit_message>
<xml_diff>
--- a/croatia/transformations/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
+++ b/croatia/transformations/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
@@ -2129,73 +2129,73 @@
         <v>0.89</v>
       </c>
       <c r="V2">
-        <v>0.8641666666666667</v>
+        <v>0.88</v>
       </c>
       <c r="W2">
-        <v>0.8391666666666666</v>
+        <v>0.8539130434782609</v>
       </c>
       <c r="X2">
-        <v>0.8149999999999999</v>
+        <v>0.8286956521739131</v>
       </c>
       <c r="Y2">
-        <v>0.7916666666666667</v>
+        <v>0.8043478260869564</v>
       </c>
       <c r="Z2">
-        <v>0.7691666666666666</v>
+        <v>0.7808695652173914</v>
       </c>
       <c r="AA2">
-        <v>0.7474999999999999</v>
+        <v>0.7582608695652174</v>
       </c>
       <c r="AB2">
-        <v>0.7266666666666666</v>
+        <v>0.7365217391304347</v>
       </c>
       <c r="AC2">
-        <v>0.7066666666666668</v>
+        <v>0.7156521739130435</v>
       </c>
       <c r="AD2">
-        <v>0.6875</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="AE2">
-        <v>0.6691666666666667</v>
+        <v>0.6765217391304349</v>
       </c>
       <c r="AF2">
-        <v>0.6516666666666667</v>
+        <v>0.6582608695652175</v>
       </c>
       <c r="AG2">
-        <v>0.635</v>
+        <v>0.6408695652173912</v>
       </c>
       <c r="AH2">
-        <v>0.6191666666666666</v>
+        <v>0.6243478260869566</v>
       </c>
       <c r="AI2">
-        <v>0.6041666666666667</v>
+        <v>0.6086956521739131</v>
       </c>
       <c r="AJ2">
-        <v>0.59</v>
+        <v>0.5939130434782609</v>
       </c>
       <c r="AK2">
-        <v>0.5766666666666667</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AL2">
-        <v>0.5641666666666667</v>
+        <v>0.5669565217391305</v>
       </c>
       <c r="AM2">
-        <v>0.5525</v>
+        <v>0.5547826086956522</v>
       </c>
       <c r="AN2">
-        <v>0.5416666666666666</v>
+        <v>0.5434782608695652</v>
       </c>
       <c r="AO2">
-        <v>0.5333333333333333</v>
+        <v>0.5347826086956522</v>
       </c>
       <c r="AP2">
-        <v>0.525</v>
+        <v>0.5260869565217391</v>
       </c>
       <c r="AQ2">
-        <v>0.5166666666666667</v>
+        <v>0.5173913043478261</v>
       </c>
       <c r="AR2">
-        <v>0.5083333333333333</v>
+        <v>0.508695652173913</v>
       </c>
       <c r="AS2">
         <v>0.5</v>

</xml_diff>

<commit_message>
Update README with file structure details, modify Croatia input file name, and enhance GeneralUtils to handle missing columns more gracefully
</commit_message>
<xml_diff>
--- a/croatia/transformations/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
+++ b/croatia/transformations/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
@@ -839,112 +839,112 @@
         <v>0.5</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AA4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AB4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AC4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AD4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AE4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AF4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AG4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AH4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AI4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AJ4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AK4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AL4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AM4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AN4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AO4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AP4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AQ4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AR4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
       <c r="AS4">
-        <v>1</v>
+        <v>1.63369506732604</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -961,112 +961,112 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="K5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="L5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="M5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="N5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="O5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="P5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="Q5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="R5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="S5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="T5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="U5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="V5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="W5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="X5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="Y5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="Z5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AA5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AB5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AC5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AD5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AE5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AF5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AG5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AH5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AI5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AJ5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AK5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AL5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AM5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AN5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AO5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AP5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AQ5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AR5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
       <c r="AS5">
-        <v>-0.1</v>
+        <v>-0.0317660546140297</v>
       </c>
     </row>
     <row r="6" spans="1:45">

</xml_diff>

<commit_message>
Update Croatia input file name and improve column comparison messages in GeneralUtils
</commit_message>
<xml_diff>
--- a/croatia/transformations/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
+++ b/croatia/transformations/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
@@ -595,112 +595,112 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>74.90263249</v>
+        <v>45.65220107373895</v>
       </c>
       <c r="K2">
-        <v>76.146574058</v>
+        <v>46.41036762541388</v>
       </c>
       <c r="L2">
-        <v>77.390515626</v>
+        <v>47.16853417708881</v>
       </c>
       <c r="M2">
-        <v>78.63445719400001</v>
+        <v>47.92670072876376</v>
       </c>
       <c r="N2">
-        <v>79.878398762</v>
+        <v>48.68486728043868</v>
       </c>
       <c r="O2">
-        <v>81.12234033</v>
+        <v>49.44303383211361</v>
       </c>
       <c r="P2">
-        <v>91.70162115181461</v>
+        <v>55.89097083028935</v>
       </c>
       <c r="Q2">
-        <v>98.14570133448539</v>
+        <v>59.81855567550635</v>
       </c>
       <c r="R2">
-        <v>101.149814878473</v>
+        <v>61.64952464147393</v>
       </c>
       <c r="S2">
-        <v>104.93031569709</v>
+        <v>63.95369176876388</v>
       </c>
       <c r="T2">
-        <v>107.960337233361</v>
+        <v>65.80045132624767</v>
       </c>
       <c r="U2">
-        <v>110.885479180297</v>
+        <v>67.58328810903468</v>
       </c>
       <c r="V2">
-        <v>114.018780813695</v>
+        <v>69.49299557107426</v>
       </c>
       <c r="W2">
-        <v>117.204024411867</v>
+        <v>71.43436099947894</v>
       </c>
       <c r="X2">
-        <v>120.148448626099</v>
+        <v>73.22895007874062</v>
       </c>
       <c r="Y2">
-        <v>123.089207013466</v>
+        <v>75.02130488319007</v>
       </c>
       <c r="Z2">
-        <v>126.116929870647</v>
+        <v>76.86666342502818</v>
       </c>
       <c r="AA2">
-        <v>128.857962569133</v>
+        <v>78.53728796439511</v>
       </c>
       <c r="AB2">
-        <v>131.229905402076</v>
+        <v>79.9829569288255</v>
       </c>
       <c r="AC2">
-        <v>133.593328177427</v>
+        <v>81.4234330266046</v>
       </c>
       <c r="AD2">
-        <v>136.179214668483</v>
+        <v>82.99949792738515</v>
       </c>
       <c r="AE2">
-        <v>138.833778711439</v>
+        <v>84.61742092185833</v>
       </c>
       <c r="AF2">
-        <v>141.405522676758</v>
+        <v>86.18486613322112</v>
       </c>
       <c r="AG2">
-        <v>143.845647663418</v>
+        <v>87.67209125245746</v>
       </c>
       <c r="AH2">
-        <v>146.241614194161</v>
+        <v>89.13240235490146</v>
       </c>
       <c r="AI2">
-        <v>148.611295516232</v>
+        <v>90.57669295724192</v>
       </c>
       <c r="AJ2">
-        <v>150.949593471355</v>
+        <v>92.00185579690366</v>
       </c>
       <c r="AK2">
-        <v>153.20498802718</v>
+        <v>93.37649006996322</v>
       </c>
       <c r="AL2">
-        <v>155.37454722451</v>
+        <v>94.69880878461068</v>
       </c>
       <c r="AM2">
-        <v>157.464554836471</v>
+        <v>95.97264182058078</v>
       </c>
       <c r="AN2">
-        <v>159.527098209995</v>
+        <v>97.22973575281335</v>
       </c>
       <c r="AO2">
-        <v>161.555103662975</v>
+        <v>98.46577926210448</v>
       </c>
       <c r="AP2">
-        <v>163.520436820417</v>
+        <v>99.66362480501522</v>
       </c>
       <c r="AQ2">
-        <v>165.441616349941</v>
+        <v>100.8345592737375</v>
       </c>
       <c r="AR2">
-        <v>167.307095578604</v>
+        <v>101.9715451180892</v>
       </c>
       <c r="AS2">
-        <v>169.124074226625</v>
+        <v>103.0789704758992</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -839,112 +839,112 @@
         <v>0.5</v>
       </c>
       <c r="J4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="Q4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="S4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="V4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="W4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="X4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="Y4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AA4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AC4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AD4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AE4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AF4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AG4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AH4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AI4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AJ4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AK4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AL4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AM4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AN4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AO4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AP4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AQ4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AR4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
       <c r="AS4">
-        <v>1.63369506732604</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -961,112 +961,112 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="K5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="L5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="M5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="N5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="O5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="P5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="Q5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="R5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="S5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="T5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="U5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="V5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="W5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="X5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="Y5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="Z5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AA5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AB5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AC5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AD5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AE5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AF5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AG5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AH5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AI5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AJ5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AK5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AL5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AM5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AN5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AO5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AP5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AQ5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AR5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
       <c r="AS5">
-        <v>-0.0317660546140297</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="6" spans="1:45">
@@ -1089,109 +1089,109 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>0.87</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>0.86</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>0.82</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>0.8100000000000001</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>0.79</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="AG6">
-        <v>0.77</v>
+        <v>1</v>
       </c>
       <c r="AH6">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>0.74</v>
+        <v>1</v>
       </c>
       <c r="AK6">
-        <v>0.73</v>
+        <v>1</v>
       </c>
       <c r="AL6">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="AM6">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="AN6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AO6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AP6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AQ6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AR6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AS6">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -2096,106 +2096,106 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="S2">
-        <v>0.91</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="W2">
-        <v>0.8539130434782609</v>
+        <v>0.9782608695652174</v>
       </c>
       <c r="X2">
-        <v>0.8286956521739131</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="Y2">
-        <v>0.8043478260869564</v>
+        <v>0.9347826086956521</v>
       </c>
       <c r="Z2">
-        <v>0.7808695652173914</v>
+        <v>0.9130434782608696</v>
       </c>
       <c r="AA2">
-        <v>0.7582608695652174</v>
+        <v>0.891304347826087</v>
       </c>
       <c r="AB2">
-        <v>0.7365217391304347</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="AC2">
-        <v>0.7156521739130435</v>
+        <v>0.8478260869565217</v>
       </c>
       <c r="AD2">
+        <v>0.8260869565217391</v>
+      </c>
+      <c r="AE2">
+        <v>0.8043478260869565</v>
+      </c>
+      <c r="AF2">
+        <v>0.7826086956521739</v>
+      </c>
+      <c r="AG2">
+        <v>0.7608695652173914</v>
+      </c>
+      <c r="AH2">
+        <v>0.7391304347826086</v>
+      </c>
+      <c r="AI2">
+        <v>0.7173913043478262</v>
+      </c>
+      <c r="AJ2">
         <v>0.6956521739130435</v>
       </c>
-      <c r="AE2">
-        <v>0.6765217391304349</v>
-      </c>
-      <c r="AF2">
-        <v>0.6582608695652175</v>
-      </c>
-      <c r="AG2">
-        <v>0.6408695652173912</v>
-      </c>
-      <c r="AH2">
-        <v>0.6243478260869566</v>
-      </c>
-      <c r="AI2">
+      <c r="AK2">
+        <v>0.6739130434782609</v>
+      </c>
+      <c r="AL2">
+        <v>0.6521739130434783</v>
+      </c>
+      <c r="AM2">
+        <v>0.6304347826086957</v>
+      </c>
+      <c r="AN2">
         <v>0.6086956521739131</v>
       </c>
-      <c r="AJ2">
-        <v>0.5939130434782609</v>
-      </c>
-      <c r="AK2">
-        <v>0.5800000000000001</v>
-      </c>
-      <c r="AL2">
-        <v>0.5669565217391305</v>
-      </c>
-      <c r="AM2">
-        <v>0.5547826086956522</v>
-      </c>
-      <c r="AN2">
+      <c r="AO2">
+        <v>0.5869565217391304</v>
+      </c>
+      <c r="AP2">
+        <v>0.5652173913043479</v>
+      </c>
+      <c r="AQ2">
         <v>0.5434782608695652</v>
       </c>
-      <c r="AO2">
-        <v>0.5347826086956522</v>
-      </c>
-      <c r="AP2">
-        <v>0.5260869565217391</v>
-      </c>
-      <c r="AQ2">
-        <v>0.5173913043478261</v>
-      </c>
       <c r="AR2">
-        <v>0.508695652173913</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="AS2">
         <v>0.5</v>

</xml_diff>